<commit_message>
Cambios en el PID
</commit_message>
<xml_diff>
--- a/I2C_14.35.32_Mar.22.2023.xlsx
+++ b/I2C_14.35.32_Mar.22.2023.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G174"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6867,6 +6867,228 @@
         </is>
       </c>
     </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>14.55.27</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>5.94</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>9.849</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>8.074</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>12.33</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>6.72</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>14.55.35</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>5.94</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>9.849</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>8.07</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>12.23</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>6.72</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>14.55.43</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>5.938</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>9.85</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>8.069</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>12.31</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>6.7</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>14.55.51</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>5.937</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>9.85</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>8.067</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>12.29</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>6.71</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>14.55.58</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>5.937</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>9.85</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>8.066</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>12.35</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>6.71</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>14.56.06</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>5.935</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>9.849</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>8.063</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>12.25</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>6.71</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>